<commit_message>
Updating upto 70 series scenarios, modyifying Page Object Model and refracting Automation code
</commit_message>
<xml_diff>
--- a/SpecFramework/FeatureFiles/DataResources/TridTestDataWithAllScenarios.xlsx
+++ b/SpecFramework/FeatureFiles/DataResources/TridTestDataWithAllScenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="599" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="599" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PrepaidCharges" sheetId="8" r:id="rId1"/>
@@ -6954,7 +6954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="G11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9922,8 +9922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>